<commit_message>
team member report update and removal of irrelevant docs
</commit_message>
<xml_diff>
--- a/documents/Deliverable_3/FlyingMongeese_Deliverable_3_Team_Member_Report.xlsx
+++ b/documents/Deliverable_3/FlyingMongeese_Deliverable_3_Team_Member_Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cadew\Documents\GitHub\Software2project\documents\Deliverable_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aaron\Documents\GitHub\Software2project\documents\Deliverable_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA30E29-4EDB-4AEB-8EA3-60D937C898D6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2A5C41-6577-4AAA-886E-1B118686D0D6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mayur" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="129">
   <si>
     <t>Week of</t>
   </si>
@@ -418,6 +418,18 @@
   </si>
   <si>
     <t>Sped up backend by breaking down the updates into more fundamental parts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Various updates to existing and newly created documents </t>
+  </si>
+  <si>
+    <t>Update existing and newly created documents</t>
+  </si>
+  <si>
+    <t>Circumventing issue by remote desktop'ing into a Windows 10 machine with successfully configured and functional database</t>
+  </si>
+  <si>
+    <t>MySQL database on Mac OS 10.13 still persists, possibly due to age of laptop</t>
   </si>
 </sst>
 </file>
@@ -944,19 +956,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="C29" sqref="C29:D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.453125" customWidth="1"/>
-    <col min="2" max="2" width="34.54296875" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" customWidth="1"/>
-    <col min="4" max="4" width="33.453125" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
@@ -964,7 +976,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>18</v>
       </c>
@@ -974,7 +986,7 @@
       </c>
       <c r="D2" s="21"/>
     </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -988,7 +1000,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1002,7 +1014,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1016,7 +1028,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1030,7 +1042,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -1044,7 +1056,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -1058,13 +1070,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
@@ -1072,7 +1084,7 @@
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
     </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
@@ -1082,7 +1094,7 @@
       </c>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -1096,7 +1108,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
@@ -1110,7 +1122,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -1124,7 +1136,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -1138,7 +1150,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
@@ -1152,7 +1164,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
@@ -1166,13 +1178,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>7</v>
       </c>
@@ -1180,7 +1192,7 @@
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
     </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
@@ -1190,7 +1202,7 @@
       </c>
       <c r="D20" s="21"/>
     </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>1</v>
       </c>
@@ -1204,7 +1216,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -1218,7 +1230,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -1232,7 +1244,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -1246,7 +1258,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
@@ -1260,7 +1272,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
@@ -1274,13 +1286,13 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>10</v>
       </c>
@@ -1288,7 +1300,7 @@
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
     </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>109</v>
       </c>
@@ -1298,7 +1310,7 @@
       </c>
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>1</v>
       </c>
@@ -1312,7 +1324,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>2</v>
       </c>
@@ -1322,7 +1334,7 @@
       </c>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -1332,7 +1344,7 @@
       </c>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -1342,7 +1354,7 @@
       </c>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>5</v>
       </c>
@@ -1352,7 +1364,7 @@
       </c>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>6</v>
       </c>
@@ -1362,13 +1374,13 @@
       </c>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>11</v>
       </c>
@@ -1376,7 +1388,7 @@
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
     </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
         <v>0</v>
       </c>
@@ -1386,7 +1398,7 @@
       </c>
       <c r="D38" s="21"/>
     </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>1</v>
       </c>
@@ -1400,7 +1412,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>2</v>
       </c>
@@ -1410,7 +1422,7 @@
       </c>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -1420,7 +1432,7 @@
       </c>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -1430,7 +1442,7 @@
       </c>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>5</v>
       </c>
@@ -1440,7 +1452,7 @@
       </c>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>6</v>
       </c>
@@ -1450,13 +1462,13 @@
       </c>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
     </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>12</v>
       </c>
@@ -1464,7 +1476,7 @@
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
     </row>
-    <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>0</v>
       </c>
@@ -1474,7 +1486,7 @@
       </c>
       <c r="D47" s="21"/>
     </row>
-    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>1</v>
       </c>
@@ -1488,7 +1500,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>2</v>
       </c>
@@ -1498,7 +1510,7 @@
       </c>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -1508,7 +1520,7 @@
       </c>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -1518,7 +1530,7 @@
       </c>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>5</v>
       </c>
@@ -1528,7 +1540,7 @@
       </c>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>6</v>
       </c>
@@ -1540,622 +1552,9 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:D29"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D53"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:D29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="25.54296875" customWidth="1"/>
-    <col min="2" max="2" width="29.54296875" customWidth="1"/>
-    <col min="3" max="3" width="26.453125" customWidth="1"/>
-    <col min="4" max="4" width="27.54296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="21"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="21"/>
-    </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A19" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="21"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="62" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A25" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-    </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A28" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="D29" s="21"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="11"/>
-    </row>
-    <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="11"/>
-    </row>
-    <row r="33" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="11"/>
-    </row>
-    <row r="34" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="11"/>
-    </row>
-    <row r="35" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="11"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-    </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A37" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-    </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" s="21"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="11"/>
-    </row>
-    <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" s="11"/>
-    </row>
-    <row r="42" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="11"/>
-    </row>
-    <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="11"/>
-    </row>
-    <row r="44" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="11"/>
-    </row>
-    <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-    </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A46" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-    </row>
-    <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="21"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D49" s="11"/>
-    </row>
-    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D50" s="11"/>
-    </row>
-    <row r="51" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="11"/>
-    </row>
-    <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="11"/>
-    </row>
-    <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="18">
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -2168,12 +1567,625 @@
     <mergeCell ref="A46:D46"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D53"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="11"/>
+    </row>
+    <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="11"/>
+    </row>
+    <row r="33" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="11"/>
+      <c r="C33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="11"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="11"/>
+      <c r="C34" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="11"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="20"/>
+      <c r="C38" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="11"/>
+    </row>
+    <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="11"/>
+    </row>
+    <row r="42" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="11"/>
+      <c r="C42" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="11"/>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="11"/>
+      <c r="C43" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="11"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="11"/>
+      <c r="C44" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="20"/>
+      <c r="C47" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="11"/>
+      <c r="C49" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="11"/>
+    </row>
+    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="11"/>
+      <c r="C50" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="11"/>
+    </row>
+    <row r="51" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="11"/>
+      <c r="C51" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="11"/>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="11"/>
+      <c r="C52" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="11"/>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" s="11"/>
+      <c r="C53" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2183,19 +2195,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A29" sqref="A29:B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
-    <col min="2" max="2" width="29.453125" customWidth="1"/>
-    <col min="3" max="3" width="20.54296875" customWidth="1"/>
-    <col min="4" max="4" width="34.54296875" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
@@ -2203,7 +2215,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>18</v>
       </c>
@@ -2213,7 +2225,7 @@
       </c>
       <c r="D2" s="21"/>
     </row>
-    <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -2227,7 +2239,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -2241,7 +2253,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -2257,7 +2269,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -2273,7 +2285,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -2289,7 +2301,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -2303,13 +2315,13 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
@@ -2317,7 +2329,7 @@
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
     </row>
-    <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
@@ -2327,7 +2339,7 @@
       </c>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -2341,7 +2353,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
@@ -2355,7 +2367,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -2371,7 +2383,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -2387,7 +2399,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
@@ -2403,7 +2415,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
@@ -2419,13 +2431,13 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
     </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>7</v>
       </c>
@@ -2433,7 +2445,7 @@
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
     </row>
-    <row r="20" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
@@ -2443,7 +2455,7 @@
       </c>
       <c r="D20" s="21"/>
     </row>
-    <row r="21" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>1</v>
       </c>
@@ -2457,7 +2469,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -2471,7 +2483,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -2485,7 +2497,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -2499,7 +2511,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
@@ -2513,7 +2525,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
@@ -2527,13 +2539,13 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
     </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>10</v>
       </c>
@@ -2541,7 +2553,7 @@
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
     </row>
-    <row r="29" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>109</v>
       </c>
@@ -2551,7 +2563,7 @@
       </c>
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>1</v>
       </c>
@@ -2565,7 +2577,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>2</v>
       </c>
@@ -2577,7 +2589,7 @@
       </c>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -2589,7 +2601,7 @@
       </c>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -2601,7 +2613,7 @@
       </c>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>5</v>
       </c>
@@ -2613,7 +2625,7 @@
       </c>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>6</v>
       </c>
@@ -2625,13 +2637,13 @@
       </c>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>11</v>
       </c>
@@ -2639,7 +2651,7 @@
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
     </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
         <v>0</v>
       </c>
@@ -2649,7 +2661,7 @@
       </c>
       <c r="D38" s="21"/>
     </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>1</v>
       </c>
@@ -2663,7 +2675,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>2</v>
       </c>
@@ -2673,7 +2685,7 @@
       </c>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -2683,7 +2695,7 @@
       </c>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -2693,7 +2705,7 @@
       </c>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>5</v>
       </c>
@@ -2703,7 +2715,7 @@
       </c>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>6</v>
       </c>
@@ -2713,13 +2725,13 @@
       </c>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
     </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>12</v>
       </c>
@@ -2727,7 +2739,7 @@
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
     </row>
-    <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>0</v>
       </c>
@@ -2737,7 +2749,7 @@
       </c>
       <c r="D47" s="21"/>
     </row>
-    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>1</v>
       </c>
@@ -2751,7 +2763,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>2</v>
       </c>
@@ -2761,7 +2773,7 @@
       </c>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -2771,7 +2783,7 @@
       </c>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -2781,7 +2793,7 @@
       </c>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>5</v>
       </c>
@@ -2791,7 +2803,7 @@
       </c>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>6</v>
       </c>
@@ -2803,12 +2815,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -2821,6 +2827,12 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2830,20 +2842,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.453125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="29.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>9</v>
       </c>
@@ -2851,7 +2863,7 @@
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
     </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -2861,7 +2873,7 @@
       </c>
       <c r="D2" s="21"/>
     </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -2875,7 +2887,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -2889,7 +2901,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -2903,7 +2915,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -2917,7 +2929,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -2931,7 +2943,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -2945,13 +2957,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>8</v>
       </c>
@@ -2959,7 +2971,7 @@
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
     </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
@@ -2969,7 +2981,7 @@
       </c>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
@@ -2983,7 +2995,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
@@ -2997,7 +3009,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -3011,7 +3023,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -3025,7 +3037,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -3039,7 +3051,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>6</v>
       </c>
@@ -3053,13 +3065,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>7</v>
       </c>
@@ -3067,7 +3079,7 @@
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
     </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
@@ -3077,7 +3089,7 @@
       </c>
       <c r="D20" s="21"/>
     </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>1</v>
       </c>
@@ -3091,7 +3103,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -3105,7 +3117,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -3119,7 +3131,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -3133,7 +3145,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -3147,7 +3159,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -3161,13 +3173,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>10</v>
       </c>
@@ -3175,7 +3187,7 @@
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
     </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>109</v>
       </c>
@@ -3185,7 +3197,7 @@
       </c>
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
@@ -3199,7 +3211,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>2</v>
       </c>
@@ -3213,7 +3225,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -3227,7 +3239,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -3241,7 +3253,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -3255,7 +3267,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -3269,13 +3281,13 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>11</v>
       </c>
@@ -3283,7 +3295,7 @@
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
     </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
         <v>114</v>
       </c>
@@ -3293,7 +3305,7 @@
       </c>
       <c r="D38" s="21"/>
     </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>1</v>
       </c>
@@ -3307,63 +3319,83 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B40" s="4"/>
+      <c r="B40" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="C40" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D40" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="4"/>
+      <c r="B41" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="C41" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="D41" s="17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="4"/>
+      <c r="B42" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="C42" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D42" s="4"/>
-    </row>
-    <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D42" s="17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="4"/>
+      <c r="B43" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="C43" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D43" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="4"/>
+      <c r="B44" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="C44" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D44" s="17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
         <v>12</v>
       </c>
@@ -3371,7 +3403,7 @@
       <c r="C46" s="22"/>
       <c r="D46" s="22"/>
     </row>
-    <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
         <v>0</v>
       </c>
@@ -3381,7 +3413,7 @@
       </c>
       <c r="D47" s="21"/>
     </row>
-    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>1</v>
       </c>
@@ -3395,17 +3427,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B49" s="4"/>
+      <c r="B49" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="C49" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D49" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -3415,7 +3451,7 @@
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -3425,7 +3461,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>5</v>
       </c>
@@ -3435,7 +3471,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>6</v>
       </c>
@@ -3447,12 +3483,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -3465,6 +3495,12 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3475,19 +3511,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="2" max="2" width="40.81640625" customWidth="1"/>
-    <col min="3" max="3" width="22.54296875" customWidth="1"/>
-    <col min="4" max="4" width="40.54296875" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>9</v>
       </c>
@@ -3495,7 +3531,7 @@
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
     </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -3505,7 +3541,7 @@
       </c>
       <c r="D2" s="21"/>
     </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -3519,7 +3555,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -3533,7 +3569,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -3547,7 +3583,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -3561,7 +3597,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -3575,7 +3611,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -3589,13 +3625,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>8</v>
       </c>
@@ -3603,7 +3639,7 @@
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
     </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
@@ -3613,7 +3649,7 @@
       </c>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
@@ -3627,7 +3663,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
@@ -3641,7 +3677,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -3655,7 +3691,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="93" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -3669,7 +3705,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -3683,7 +3719,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>6</v>
       </c>
@@ -3697,13 +3733,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>7</v>
       </c>
@@ -3711,7 +3747,7 @@
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
     </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
@@ -3721,7 +3757,7 @@
       </c>
       <c r="D20" s="21"/>
     </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>1</v>
       </c>
@@ -3735,7 +3771,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -3749,7 +3785,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -3763,7 +3799,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -3777,7 +3813,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -3791,7 +3827,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -3805,13 +3841,13 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>10</v>
       </c>
@@ -3819,7 +3855,7 @@
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
     </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>109</v>
       </c>
@@ -3829,7 +3865,7 @@
       </c>
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
@@ -3843,7 +3879,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>2</v>
       </c>
@@ -3857,7 +3893,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="93" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -3871,7 +3907,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -3885,7 +3921,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -3899,7 +3935,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -3913,13 +3949,13 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>11</v>
       </c>
@@ -3927,7 +3963,7 @@
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
     </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
         <v>0</v>
       </c>
@@ -3937,7 +3973,7 @@
       </c>
       <c r="D38" s="21"/>
     </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>1</v>
       </c>
@@ -3951,7 +3987,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>2</v>
       </c>
@@ -3961,7 +3997,7 @@
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -3971,7 +4007,7 @@
       </c>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -3981,7 +4017,7 @@
       </c>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>5</v>
       </c>
@@ -3991,7 +4027,7 @@
       </c>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>6</v>
       </c>
@@ -4001,13 +4037,13 @@
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
         <v>12</v>
       </c>
@@ -4015,7 +4051,7 @@
       <c r="C46" s="22"/>
       <c r="D46" s="22"/>
     </row>
-    <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
         <v>0</v>
       </c>
@@ -4025,7 +4061,7 @@
       </c>
       <c r="D47" s="21"/>
     </row>
-    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>1</v>
       </c>
@@ -4039,7 +4075,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>2</v>
       </c>
@@ -4049,7 +4085,7 @@
       </c>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -4059,7 +4095,7 @@
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -4069,7 +4105,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>5</v>
       </c>
@@ -4079,7 +4115,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>6</v>
       </c>
@@ -4091,12 +4127,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -4109,6 +4139,12 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4119,19 +4155,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.54296875" customWidth="1"/>
-    <col min="2" max="2" width="40.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.54296875" customWidth="1"/>
-    <col min="4" max="4" width="40.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
@@ -4139,7 +4175,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -4149,7 +4185,7 @@
       </c>
       <c r="D2" s="21"/>
     </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -4163,7 +4199,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -4177,7 +4213,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -4191,7 +4227,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -4205,7 +4241,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -4219,7 +4255,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -4233,13 +4269,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>8</v>
       </c>
@@ -4247,7 +4283,7 @@
       <c r="C10" s="24"/>
       <c r="D10" s="25"/>
     </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
@@ -4257,7 +4293,7 @@
       </c>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -4271,7 +4307,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
@@ -4285,7 +4321,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -4299,7 +4335,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -4313,7 +4349,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
@@ -4327,7 +4363,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
@@ -4341,13 +4377,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>7</v>
       </c>
@@ -4355,7 +4391,7 @@
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
     </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
@@ -4365,7 +4401,7 @@
       </c>
       <c r="D20" s="21"/>
     </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>1</v>
       </c>
@@ -4379,7 +4415,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -4393,7 +4429,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -4407,7 +4443,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -4421,7 +4457,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
@@ -4435,7 +4471,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
@@ -4449,13 +4485,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>10</v>
       </c>
@@ -4463,7 +4499,7 @@
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
     </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>109</v>
       </c>
@@ -4473,7 +4509,7 @@
       </c>
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>1</v>
       </c>
@@ -4487,7 +4523,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>2</v>
       </c>
@@ -4497,7 +4533,7 @@
       </c>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -4507,7 +4543,7 @@
       </c>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -4517,7 +4553,7 @@
       </c>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>5</v>
       </c>
@@ -4527,7 +4563,7 @@
       </c>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>6</v>
       </c>
@@ -4537,13 +4573,13 @@
       </c>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>11</v>
       </c>
@@ -4551,7 +4587,7 @@
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
     </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
         <v>18</v>
       </c>
@@ -4561,7 +4597,7 @@
       </c>
       <c r="D38" s="21"/>
     </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>1</v>
       </c>
@@ -4575,7 +4611,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>2</v>
       </c>
@@ -4585,7 +4621,7 @@
       </c>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -4595,7 +4631,7 @@
       </c>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -4605,7 +4641,7 @@
       </c>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>5</v>
       </c>
@@ -4615,7 +4651,7 @@
       </c>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>6</v>
       </c>
@@ -4625,13 +4661,13 @@
       </c>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
     </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>11</v>
       </c>
@@ -4639,7 +4675,7 @@
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
     </row>
-    <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>18</v>
       </c>
@@ -4649,7 +4685,7 @@
       </c>
       <c r="D47" s="21"/>
     </row>
-    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>1</v>
       </c>
@@ -4663,7 +4699,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>2</v>
       </c>
@@ -4673,7 +4709,7 @@
       </c>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -4683,7 +4719,7 @@
       </c>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -4693,7 +4729,7 @@
       </c>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>5</v>
       </c>
@@ -4703,7 +4739,7 @@
       </c>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>6</v>
       </c>
@@ -4715,12 +4751,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -4733,6 +4763,12 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update team member report
</commit_message>
<xml_diff>
--- a/documents/Deliverable_3/FlyingMongeese_Deliverable_3_Team_Member_Report.xlsx
+++ b/documents/Deliverable_3/FlyingMongeese_Deliverable_3_Team_Member_Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aaron\Documents\GitHub\Software2project\documents\Deliverable_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carolyn\Documents\GitHub\Software2project\documents\Deliverable_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2A5C41-6577-4AAA-886E-1B118686D0D6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E5A042-5D10-4E48-9341-ADF72D3A7E15}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mayur" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="133">
   <si>
     <t>Week of</t>
   </si>
@@ -430,6 +430,18 @@
   </si>
   <si>
     <t>MySQL database on Mac OS 10.13 still persists, possibly due to age of laptop</t>
+  </si>
+  <si>
+    <t>developer</t>
+  </si>
+  <si>
+    <t>devloper</t>
+  </si>
+  <si>
+    <t>struggle with the choice of design pattern and architecture design</t>
+  </si>
+  <si>
+    <t>talk to professor and read material</t>
   </si>
 </sst>
 </file>
@@ -960,15 +972,15 @@
       <selection activeCell="C29" sqref="C29:D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="34.5546875" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" customWidth="1"/>
+    <col min="4" max="4" width="33.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
@@ -976,7 +988,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>18</v>
       </c>
@@ -986,7 +998,7 @@
       </c>
       <c r="D2" s="21"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1000,7 +1012,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1014,7 +1026,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1028,7 +1040,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1042,7 +1054,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -1056,7 +1068,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -1070,13 +1082,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
@@ -1084,7 +1096,7 @@
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
@@ -1094,7 +1106,7 @@
       </c>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -1108,7 +1120,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
@@ -1122,7 +1134,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -1136,7 +1148,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -1150,7 +1162,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
@@ -1164,7 +1176,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
@@ -1178,13 +1190,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>7</v>
       </c>
@@ -1192,7 +1204,7 @@
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
@@ -1202,7 +1214,7 @@
       </c>
       <c r="D20" s="21"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>1</v>
       </c>
@@ -1216,7 +1228,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -1230,7 +1242,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -1244,7 +1256,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -1258,7 +1270,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
@@ -1272,7 +1284,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
@@ -1286,13 +1298,13 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
         <v>10</v>
       </c>
@@ -1300,7 +1312,7 @@
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>109</v>
       </c>
@@ -1310,7 +1322,7 @@
       </c>
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>1</v>
       </c>
@@ -1324,7 +1336,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>2</v>
       </c>
@@ -1334,7 +1346,7 @@
       </c>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -1344,7 +1356,7 @@
       </c>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -1354,7 +1366,7 @@
       </c>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>5</v>
       </c>
@@ -1364,7 +1376,7 @@
       </c>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>6</v>
       </c>
@@ -1374,13 +1386,13 @@
       </c>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
         <v>11</v>
       </c>
@@ -1388,7 +1400,7 @@
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
         <v>0</v>
       </c>
@@ -1398,7 +1410,7 @@
       </c>
       <c r="D38" s="21"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>1</v>
       </c>
@@ -1412,7 +1424,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>2</v>
       </c>
@@ -1422,7 +1434,7 @@
       </c>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -1432,7 +1444,7 @@
       </c>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -1442,7 +1454,7 @@
       </c>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>5</v>
       </c>
@@ -1452,7 +1464,7 @@
       </c>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>6</v>
       </c>
@@ -1462,13 +1474,13 @@
       </c>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
         <v>12</v>
       </c>
@@ -1476,7 +1488,7 @@
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
         <v>0</v>
       </c>
@@ -1486,7 +1498,7 @@
       </c>
       <c r="D47" s="21"/>
     </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>1</v>
       </c>
@@ -1500,7 +1512,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>2</v>
       </c>
@@ -1510,7 +1522,7 @@
       </c>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -1520,7 +1532,7 @@
       </c>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -1530,7 +1542,7 @@
       </c>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>5</v>
       </c>
@@ -1540,7 +1552,7 @@
       </c>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>6</v>
       </c>
@@ -1552,9 +1564,622 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:D29"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D53"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="11"/>
+    </row>
+    <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="11"/>
+    </row>
+    <row r="33" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="11"/>
+      <c r="C33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="11"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="11"/>
+      <c r="C34" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="11"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="20"/>
+      <c r="C38" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="11"/>
+    </row>
+    <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="11"/>
+    </row>
+    <row r="42" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="11"/>
+      <c r="C42" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="11"/>
+    </row>
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="11"/>
+      <c r="C43" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="11"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="11"/>
+      <c r="C44" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+    </row>
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="20"/>
+      <c r="C47" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="11"/>
+      <c r="C49" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="11"/>
+    </row>
+    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="11"/>
+      <c r="C50" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="11"/>
+    </row>
+    <row r="51" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="11"/>
+      <c r="C51" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="11"/>
+    </row>
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="11"/>
+      <c r="C52" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="11"/>
+    </row>
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" s="11"/>
+      <c r="C53" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -1567,625 +2192,12 @@
     <mergeCell ref="A46:D46"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D53"/>
-  <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:D29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="21"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="21"/>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="21"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="63" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="D29" s="21"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="11"/>
-    </row>
-    <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="11"/>
-    </row>
-    <row r="33" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="11"/>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="11"/>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="11"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" s="21"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="11"/>
-    </row>
-    <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" s="11"/>
-    </row>
-    <row r="42" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="11"/>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="11"/>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="11"/>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="21"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D49" s="11"/>
-    </row>
-    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D50" s="11"/>
-    </row>
-    <row r="51" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="11"/>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="11"/>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2195,19 +2207,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A29" sqref="A29:B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="4" max="4" width="34.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
@@ -2215,7 +2227,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>18</v>
       </c>
@@ -2225,7 +2237,7 @@
       </c>
       <c r="D2" s="21"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -2239,7 +2251,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -2253,7 +2265,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -2269,7 +2281,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -2285,7 +2297,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -2301,7 +2313,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -2315,13 +2327,13 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
@@ -2329,7 +2341,7 @@
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
@@ -2339,7 +2351,7 @@
       </c>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -2353,7 +2365,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
@@ -2367,7 +2379,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -2383,7 +2395,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -2399,7 +2411,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
@@ -2415,7 +2427,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
@@ -2431,13 +2443,13 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
     </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>7</v>
       </c>
@@ -2445,7 +2457,7 @@
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
     </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
@@ -2455,7 +2467,7 @@
       </c>
       <c r="D20" s="21"/>
     </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>1</v>
       </c>
@@ -2469,7 +2481,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -2483,7 +2495,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -2497,7 +2509,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -2511,7 +2523,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
@@ -2525,7 +2537,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
@@ -2539,13 +2551,13 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
     </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
         <v>10</v>
       </c>
@@ -2553,7 +2565,7 @@
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
     </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>109</v>
       </c>
@@ -2563,7 +2575,7 @@
       </c>
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>1</v>
       </c>
@@ -2577,7 +2589,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>2</v>
       </c>
@@ -2589,7 +2601,7 @@
       </c>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -2601,7 +2613,7 @@
       </c>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -2613,7 +2625,7 @@
       </c>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>5</v>
       </c>
@@ -2625,7 +2637,7 @@
       </c>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>6</v>
       </c>
@@ -2637,13 +2649,13 @@
       </c>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="14"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
         <v>11</v>
       </c>
@@ -2651,7 +2663,7 @@
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
         <v>0</v>
       </c>
@@ -2661,7 +2673,7 @@
       </c>
       <c r="D38" s="21"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>1</v>
       </c>
@@ -2675,7 +2687,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>2</v>
       </c>
@@ -2685,7 +2697,7 @@
       </c>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -2695,7 +2707,7 @@
       </c>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -2705,7 +2717,7 @@
       </c>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>5</v>
       </c>
@@ -2715,7 +2727,7 @@
       </c>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>6</v>
       </c>
@@ -2725,13 +2737,13 @@
       </c>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
         <v>12</v>
       </c>
@@ -2739,7 +2751,7 @@
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
         <v>0</v>
       </c>
@@ -2749,7 +2761,7 @@
       </c>
       <c r="D47" s="21"/>
     </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>1</v>
       </c>
@@ -2763,7 +2775,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>2</v>
       </c>
@@ -2773,7 +2785,7 @@
       </c>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -2783,7 +2795,7 @@
       </c>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -2793,7 +2805,7 @@
       </c>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>5</v>
       </c>
@@ -2803,7 +2815,7 @@
       </c>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>6</v>
       </c>
@@ -2815,6 +2827,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -2827,12 +2845,6 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2842,20 +2854,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="29.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>9</v>
       </c>
@@ -2863,7 +2875,7 @@
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -2873,7 +2885,7 @@
       </c>
       <c r="D2" s="21"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -2887,7 +2899,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -2901,7 +2913,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -2915,7 +2927,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -2929,7 +2941,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -2943,7 +2955,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -2957,13 +2969,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>8</v>
       </c>
@@ -2971,7 +2983,7 @@
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
@@ -2981,7 +2993,7 @@
       </c>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
@@ -2995,7 +3007,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
@@ -3009,7 +3021,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -3023,7 +3035,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -3037,7 +3049,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -3051,7 +3063,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>6</v>
       </c>
@@ -3065,13 +3077,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>7</v>
       </c>
@@ -3079,7 +3091,7 @@
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
@@ -3089,7 +3101,7 @@
       </c>
       <c r="D20" s="21"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>1</v>
       </c>
@@ -3103,7 +3115,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -3117,7 +3129,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -3131,7 +3143,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -3145,7 +3157,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -3159,7 +3171,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -3173,13 +3185,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>10</v>
       </c>
@@ -3187,7 +3199,7 @@
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>109</v>
       </c>
@@ -3197,7 +3209,7 @@
       </c>
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
@@ -3211,7 +3223,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>2</v>
       </c>
@@ -3225,7 +3237,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -3239,7 +3251,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -3253,7 +3265,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -3267,7 +3279,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -3281,13 +3293,13 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="22" t="s">
         <v>11</v>
       </c>
@@ -3295,7 +3307,7 @@
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="21" t="s">
         <v>114</v>
       </c>
@@ -3305,7 +3317,7 @@
       </c>
       <c r="D38" s="21"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>1</v>
       </c>
@@ -3319,7 +3331,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>2</v>
       </c>
@@ -3333,7 +3345,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -3347,7 +3359,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -3361,7 +3373,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>5</v>
       </c>
@@ -3375,7 +3387,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>6</v>
       </c>
@@ -3389,13 +3401,13 @@
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="22" t="s">
         <v>12</v>
       </c>
@@ -3403,7 +3415,7 @@
       <c r="C46" s="22"/>
       <c r="D46" s="22"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="21" t="s">
         <v>0</v>
       </c>
@@ -3413,7 +3425,7 @@
       </c>
       <c r="D47" s="21"/>
     </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>1</v>
       </c>
@@ -3427,7 +3439,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>2</v>
       </c>
@@ -3441,7 +3453,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -3451,7 +3463,7 @@
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -3461,7 +3473,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>5</v>
       </c>
@@ -3471,7 +3483,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>6</v>
       </c>
@@ -3483,6 +3495,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -3495,12 +3513,6 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3515,15 +3527,15 @@
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="40.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="40.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="40.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>9</v>
       </c>
@@ -3531,7 +3543,7 @@
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -3541,7 +3553,7 @@
       </c>
       <c r="D2" s="21"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -3555,7 +3567,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -3569,7 +3581,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -3583,7 +3595,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -3597,7 +3609,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -3611,7 +3623,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -3625,13 +3637,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>8</v>
       </c>
@@ -3639,7 +3651,7 @@
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
@@ -3649,7 +3661,7 @@
       </c>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
@@ -3663,7 +3675,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
@@ -3677,7 +3689,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="78" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -3691,7 +3703,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -3705,7 +3717,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -3719,7 +3731,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>6</v>
       </c>
@@ -3733,13 +3745,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>7</v>
       </c>
@@ -3747,7 +3759,7 @@
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
@@ -3757,7 +3769,7 @@
       </c>
       <c r="D20" s="21"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>1</v>
       </c>
@@ -3771,7 +3783,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -3785,7 +3797,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -3799,7 +3811,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -3813,7 +3825,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -3827,7 +3839,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -3841,13 +3853,13 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>10</v>
       </c>
@@ -3855,7 +3867,7 @@
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>109</v>
       </c>
@@ -3865,7 +3877,7 @@
       </c>
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
@@ -3879,7 +3891,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>2</v>
       </c>
@@ -3893,7 +3905,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -3907,7 +3919,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="78" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -3921,7 +3933,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="78" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -3935,7 +3947,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -3949,13 +3961,13 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="22" t="s">
         <v>11</v>
       </c>
@@ -3963,7 +3975,7 @@
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="21" t="s">
         <v>0</v>
       </c>
@@ -3973,7 +3985,7 @@
       </c>
       <c r="D38" s="21"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>1</v>
       </c>
@@ -3987,7 +3999,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>2</v>
       </c>
@@ -3997,7 +4009,7 @@
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -4007,7 +4019,7 @@
       </c>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -4017,7 +4029,7 @@
       </c>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>5</v>
       </c>
@@ -4027,7 +4039,7 @@
       </c>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>6</v>
       </c>
@@ -4037,13 +4049,13 @@
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="22" t="s">
         <v>12</v>
       </c>
@@ -4051,7 +4063,7 @@
       <c r="C46" s="22"/>
       <c r="D46" s="22"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="21" t="s">
         <v>0</v>
       </c>
@@ -4061,7 +4073,7 @@
       </c>
       <c r="D47" s="21"/>
     </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>1</v>
       </c>
@@ -4075,7 +4087,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>2</v>
       </c>
@@ -4085,7 +4097,7 @@
       </c>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -4095,7 +4107,7 @@
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -4105,7 +4117,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>5</v>
       </c>
@@ -4115,7 +4127,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>6</v>
       </c>
@@ -4127,6 +4139,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -4139,12 +4157,6 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4155,19 +4167,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
-    <col min="2" max="2" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" customWidth="1"/>
+    <col min="4" max="4" width="40.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
@@ -4175,7 +4187,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -4185,7 +4197,7 @@
       </c>
       <c r="D2" s="21"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -4199,7 +4211,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -4213,7 +4225,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -4227,7 +4239,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -4241,7 +4253,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -4255,7 +4267,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -4269,13 +4281,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>8</v>
       </c>
@@ -4283,7 +4295,7 @@
       <c r="C10" s="24"/>
       <c r="D10" s="25"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
@@ -4293,7 +4305,7 @@
       </c>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -4307,7 +4319,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
@@ -4321,7 +4333,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -4335,7 +4347,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -4349,7 +4361,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
@@ -4363,7 +4375,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
@@ -4377,13 +4389,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>7</v>
       </c>
@@ -4391,7 +4403,7 @@
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
@@ -4401,7 +4413,7 @@
       </c>
       <c r="D20" s="21"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>1</v>
       </c>
@@ -4415,7 +4427,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -4429,7 +4441,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -4443,7 +4455,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -4457,7 +4469,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
@@ -4471,7 +4483,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
@@ -4485,13 +4497,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
         <v>10</v>
       </c>
@@ -4499,7 +4511,7 @@
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>109</v>
       </c>
@@ -4509,7 +4521,7 @@
       </c>
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>1</v>
       </c>
@@ -4523,63 +4535,83 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="8"/>
+      <c r="B31" s="8" t="s">
+        <v>129</v>
+      </c>
       <c r="C31" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="8"/>
-    </row>
-    <row r="32" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="8"/>
+      <c r="B32" s="8" t="s">
+        <v>125</v>
+      </c>
       <c r="C32" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="8"/>
-    </row>
-    <row r="33" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="8"/>
+      <c r="B33" s="18" t="s">
+        <v>126</v>
+      </c>
       <c r="C33" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="8"/>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D33" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="8"/>
+      <c r="B34" s="8" t="s">
+        <v>131</v>
+      </c>
       <c r="C34" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="8"/>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D34" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="8"/>
+      <c r="B35" s="8" t="s">
+        <v>132</v>
+      </c>
       <c r="C35" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D35" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
         <v>11</v>
       </c>
@@ -4587,7 +4619,7 @@
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
         <v>18</v>
       </c>
@@ -4597,7 +4629,7 @@
       </c>
       <c r="D38" s="21"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>1</v>
       </c>
@@ -4611,7 +4643,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>2</v>
       </c>
@@ -4621,7 +4653,7 @@
       </c>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -4631,7 +4663,7 @@
       </c>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -4641,7 +4673,7 @@
       </c>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>5</v>
       </c>
@@ -4651,7 +4683,7 @@
       </c>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>6</v>
       </c>
@@ -4661,13 +4693,13 @@
       </c>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
         <v>11</v>
       </c>
@@ -4675,7 +4707,7 @@
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
         <v>18</v>
       </c>
@@ -4685,7 +4717,7 @@
       </c>
       <c r="D47" s="21"/>
     </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>1</v>
       </c>
@@ -4699,7 +4731,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>2</v>
       </c>
@@ -4709,7 +4741,7 @@
       </c>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -4719,7 +4751,7 @@
       </c>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -4729,7 +4761,7 @@
       </c>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>5</v>
       </c>
@@ -4739,7 +4771,7 @@
       </c>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>6</v>
       </c>
@@ -4751,6 +4783,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -4763,12 +4801,6 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>